<commit_message>
Add new evidence screenshots (TC-001..TC-010) and update demo_testcases.xlsx
</commit_message>
<xml_diff>
--- a/demo_testcases.xlsx
+++ b/demo_testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kar Har Maidan Fateh!\project_option_b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FBD96C-10DF-455C-A942-F4B68701F0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A8080D-4326-457C-9BA6-379D1723A24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18448" yWindow="-2228" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
   <si>
     <t>Column1</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Functional</t>
   </si>
   <si>
-    <t>Not Run</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
@@ -277,13 +274,19 @@
   </si>
   <si>
     <t>Usability</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,13 +294,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -312,12 +329,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -326,12 +346,6 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -373,6 +387,12 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -409,20 +429,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67F46CA7-F798-4C00-B827-05105A91288F}" name="demo_testcases_csv" displayName="demo_testcases_csv" ref="A1:K12" tableType="queryTable" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67F46CA7-F798-4C00-B827-05105A91288F}" name="demo_testcases_csv" displayName="demo_testcases_csv" ref="A1:K12" tableType="queryTable" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:K12" xr:uid="{67F46CA7-F798-4C00-B827-05105A91288F}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{79A83944-4BCF-4E5E-A720-DC6F05E0F396}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{CF6E1F1A-868C-47BA-BCED-C6D801EB02F0}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{C22FF5B1-B12A-4DCD-926B-642E4C432EA6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{5FBC6895-73C5-4094-9417-E1F3EB543B01}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{3A6D2CB0-25EB-4740-8A5B-8CCF8535D5A3}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{A5A16648-25C0-401C-BB73-91B1B0BEA907}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{EFBD47CE-A199-420F-A8FC-0284F7F56ADD}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{E0C79904-BF48-4976-B6B0-D9D39F8F6F39}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{1FC2F84D-C583-4DC5-B693-08522317A2CB}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{7FD56E4E-C184-49E2-AE7D-0E966B71CFB2}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{4FCAAD74-1B12-4111-B81C-C51A93DD127A}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{79A83944-4BCF-4E5E-A720-DC6F05E0F396}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{CF6E1F1A-868C-47BA-BCED-C6D801EB02F0}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{C22FF5B1-B12A-4DCD-926B-642E4C432EA6}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{5FBC6895-73C5-4094-9417-E1F3EB543B01}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{3A6D2CB0-25EB-4740-8A5B-8CCF8535D5A3}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{A5A16648-25C0-401C-BB73-91B1B0BEA907}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{EFBD47CE-A199-420F-A8FC-0284F7F56ADD}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{E0C79904-BF48-4976-B6B0-D9D39F8F6F39}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{1FC2F84D-C583-4DC5-B693-08522317A2CB}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{7FD56E4E-C184-49E2-AE7D-0E966B71CFB2}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{4FCAAD74-1B12-4111-B81C-C51A93DD127A}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -693,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F99ABFA-0089-4DAC-96A3-6136F0E54977}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -710,7 +730,7 @@
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -781,353 +801,353 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>31</v>
+      <c r="I3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>31</v>
+      <c r="I4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>31</v>
+      <c r="I5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>31</v>
+      <c r="I6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>31</v>
+      <c r="I7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>31</v>
+      <c r="I8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>31</v>
+      <c r="I9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>31</v>
+      <c r="I10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="2" t="s">
+      <c r="G11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>31</v>
+      <c r="I11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>31</v>
+      <c r="J12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retest: Signup password validation fix verified; added video evidence and updated testcases
</commit_message>
<xml_diff>
--- a/demo_testcases.xlsx
+++ b/demo_testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kar Har Maidan Fateh!\project_option_b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A8080D-4326-457C-9BA6-379D1723A24F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA4FCE4-93EA-4AB4-A599-37F99C819CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18448" yWindow="-2228" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="80">
   <si>
     <t>Column1</t>
   </si>
@@ -277,9 +277,6 @@
   </si>
   <si>
     <t>Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -303,18 +300,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -329,15 +320,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -714,7 +702,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I6" sqref="I6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -965,8 +953,8 @@
       <c r="H7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>80</v>
+      <c r="I7" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>30</v>

</xml_diff>